<commit_message>
went through a redesign of the entire project so that rotations would work properly. Just finished most of the main animation with the turrets, and all 7 initial tank models are done.
</commit_message>
<xml_diff>
--- a/James Status Update 2.xlsx
+++ b/James Status Update 2.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
   <si>
     <t>Current Status</t>
   </si>
@@ -112,6 +114,39 @@
   </si>
   <si>
     <t>Alma 42:29 - ...and only let your [bugs] trouble you, with that trouble which shall bring you down unto [fix them].</t>
+  </si>
+  <si>
+    <t>Not much … stuck on rotations still.</t>
+  </si>
+  <si>
+    <t>Changed my focus at the moment to the models between research, so that I can progress</t>
+  </si>
+  <si>
+    <t>Actual hours since last update: 17 hours</t>
+  </si>
+  <si>
+    <t>Total Anticipated actual Hours:  258</t>
+  </si>
+  <si>
+    <t>Trying to figure out this bug with rotational movement, while moving on to the actual struture of the models.</t>
+  </si>
+  <si>
+    <t>Acts 27:41 - And falling into a place where [problems] met, they ran the [project] aground; and the forepart stuck fast, and remained unmoveable, but the hinder part was broken with the violence of the waves.</t>
+  </si>
+  <si>
+    <t>Started making the tank objects, and put a little research time into obj files.</t>
+  </si>
+  <si>
+    <t>still hammering through making models and looking a bit at rotations.</t>
+  </si>
+  <si>
+    <t>Research a bit about obj files, and decided that is not the way to go, and it would just complicate thing a bit more.</t>
+  </si>
+  <si>
+    <t>Actual hours since last update: 5 hours</t>
+  </si>
+  <si>
+    <t>Numbers 22:24 -  But the [rotational problem]stood in a path of the [James' goal] a wall being on this side, and a wall on that side.</t>
   </si>
 </sst>
 </file>
@@ -121,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +178,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,18 +280,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,11 +315,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,8 +336,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,346 +676,350 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="31" thickBot="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>41699</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>41699</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>41699</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>41765</v>
       </c>
-      <c r="G3" s="8">
-        <v>41766</v>
-      </c>
-      <c r="H3" s="8">
-        <v>41766</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="G3" s="6">
+        <v>41766</v>
+      </c>
+      <c r="H3" s="6">
+        <v>41766</v>
+      </c>
+      <c r="I3" s="7">
         <v>5</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <v>6</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16" thickBot="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8">
-        <v>41766</v>
-      </c>
-      <c r="D4" s="8">
-        <v>41766</v>
-      </c>
-      <c r="E4" s="8">
-        <v>41766</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="C4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="D4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="E4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="F4" s="6">
         <v>41768</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>41768</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>41772</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>3</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <v>3</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16" thickBot="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8">
-        <v>41766</v>
-      </c>
-      <c r="D5" s="8">
-        <v>41766</v>
-      </c>
-      <c r="E5" s="8">
-        <v>41766</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="C5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="D5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="F5" s="6">
         <v>41768</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>41768</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <v>41772</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>4</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <v>4</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>41773</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>41713</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>41713</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>41809</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>41823</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <v>41830</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>60</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <v>40.5</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>40.5</v>
       </c>
-      <c r="M6" s="12"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="16" thickBot="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>41810</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>41830</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="8">
+      <c r="E7" s="9"/>
+      <c r="F7" s="6">
         <v>41845</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>41907</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="9">
+      <c r="H7" s="9"/>
+      <c r="I7" s="7">
         <v>50</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <v>84.5</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="7">
         <v>84.5</v>
       </c>
-      <c r="M7" s="12"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>42024</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="8">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="6">
         <v>42060</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="9">
+      <c r="G8" s="11">
+        <v>42186</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="7">
         <v>47</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16" thickBot="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>42068</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="8">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="6">
         <v>42088</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="9">
+      <c r="G9" s="11">
+        <v>42214</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="7">
         <v>20</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="9">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="7">
         <v>189</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
         <v>208</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="7">
         <f>SUM(K3:K9)</f>
         <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" thickBot="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="16" thickBot="1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="16" thickBot="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="15" t="s">
         <v>21</v>
       </c>
@@ -969,10 +1035,10 @@
       <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="16" thickBot="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
@@ -986,8 +1052,8 @@
       <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:13" ht="16" thickBot="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
@@ -1001,36 +1067,948 @@
       <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:13" ht="16" thickBot="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" ht="16" thickBot="1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:K17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="A14:B16"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:K16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16" thickBot="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="16" thickBot="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="31" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>41699</v>
+      </c>
+      <c r="D3" s="6">
+        <v>41699</v>
+      </c>
+      <c r="E3" s="6">
+        <v>41699</v>
+      </c>
+      <c r="F3" s="6">
+        <v>41765</v>
+      </c>
+      <c r="G3" s="6">
+        <v>41766</v>
+      </c>
+      <c r="H3" s="6">
+        <v>41766</v>
+      </c>
+      <c r="I3" s="7">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="D4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="E4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="F4" s="6">
+        <v>41768</v>
+      </c>
+      <c r="G4" s="6">
+        <v>41768</v>
+      </c>
+      <c r="H4" s="6">
+        <v>41772</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16" thickBot="1">
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="D5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="F5" s="6">
+        <v>41768</v>
+      </c>
+      <c r="G5" s="6">
+        <v>41768</v>
+      </c>
+      <c r="H5" s="6">
+        <v>41772</v>
+      </c>
+      <c r="I5" s="7">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7">
+        <v>4</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
+        <v>41773</v>
+      </c>
+      <c r="D6" s="6">
+        <v>41713</v>
+      </c>
+      <c r="E6" s="6">
+        <v>41713</v>
+      </c>
+      <c r="F6" s="6">
+        <v>41809</v>
+      </c>
+      <c r="G6" s="6">
+        <v>41823</v>
+      </c>
+      <c r="H6" s="6">
+        <v>41830</v>
+      </c>
+      <c r="I6" s="7">
+        <v>60</v>
+      </c>
+      <c r="J6" s="7">
+        <v>40.5</v>
+      </c>
+      <c r="K6" s="7">
+        <v>40.5</v>
+      </c>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6">
+        <v>41810</v>
+      </c>
+      <c r="D7" s="6">
+        <v>41830</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="6">
+        <v>41845</v>
+      </c>
+      <c r="G7" s="6">
+        <v>41907</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="7">
+        <v>50</v>
+      </c>
+      <c r="J7" s="7">
+        <v>84.5</v>
+      </c>
+      <c r="K7" s="7">
+        <v>84.5</v>
+      </c>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6">
+        <v>42024</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="6">
+        <v>42060</v>
+      </c>
+      <c r="G8" s="11">
+        <v>42186</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="7">
+        <v>47</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6">
+        <v>42068</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="6">
+        <v>42088</v>
+      </c>
+      <c r="G9" s="11">
+        <v>42214</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="7">
+        <v>20</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="7">
+        <v>189</v>
+      </c>
+      <c r="J10" s="7">
+        <v>258</v>
+      </c>
+      <c r="K10" s="7">
+        <f>SUM(K3:K9)</f>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" thickBot="1">
+      <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" ht="16" thickBot="1">
+      <c r="A12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" ht="16" thickBot="1">
+      <c r="A13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" ht="16" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" ht="16" thickBot="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" thickBot="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" ht="31" customHeight="1" thickBot="1">
+      <c r="A17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:K17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="A14:B16"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:K16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16" thickBot="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" ht="16" thickBot="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="31" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>41699</v>
+      </c>
+      <c r="D3" s="6">
+        <v>41699</v>
+      </c>
+      <c r="E3" s="6">
+        <v>41699</v>
+      </c>
+      <c r="F3" s="6">
+        <v>41765</v>
+      </c>
+      <c r="G3" s="6">
+        <v>41766</v>
+      </c>
+      <c r="H3" s="6">
+        <v>41766</v>
+      </c>
+      <c r="I3" s="7">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="D4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="E4" s="6">
+        <v>41766</v>
+      </c>
+      <c r="F4" s="6">
+        <v>41768</v>
+      </c>
+      <c r="G4" s="6">
+        <v>41768</v>
+      </c>
+      <c r="H4" s="6">
+        <v>41772</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" thickBot="1">
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="D5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41766</v>
+      </c>
+      <c r="F5" s="6">
+        <v>41768</v>
+      </c>
+      <c r="G5" s="6">
+        <v>41768</v>
+      </c>
+      <c r="H5" s="6">
+        <v>41772</v>
+      </c>
+      <c r="I5" s="7">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7">
+        <v>4</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
+        <v>41773</v>
+      </c>
+      <c r="D6" s="6">
+        <v>41713</v>
+      </c>
+      <c r="E6" s="6">
+        <v>41713</v>
+      </c>
+      <c r="F6" s="6">
+        <v>41809</v>
+      </c>
+      <c r="G6" s="6">
+        <v>41823</v>
+      </c>
+      <c r="H6" s="6">
+        <v>41830</v>
+      </c>
+      <c r="I6" s="7">
+        <v>60</v>
+      </c>
+      <c r="J6" s="7">
+        <v>40.5</v>
+      </c>
+      <c r="K6" s="7">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6">
+        <v>41810</v>
+      </c>
+      <c r="D7" s="6">
+        <v>41830</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="6">
+        <v>41845</v>
+      </c>
+      <c r="G7" s="6">
+        <v>41907</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="7">
+        <v>50</v>
+      </c>
+      <c r="J7" s="7">
+        <v>86.5</v>
+      </c>
+      <c r="K7" s="7">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6">
+        <v>42024</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="6">
+        <v>42060</v>
+      </c>
+      <c r="G8" s="11">
+        <v>42186</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="7">
+        <v>47</v>
+      </c>
+      <c r="J8" s="7">
+        <v>60</v>
+      </c>
+      <c r="K8" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6">
+        <v>42068</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="6">
+        <v>42088</v>
+      </c>
+      <c r="G9" s="11">
+        <v>42214</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="7">
+        <v>20</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="16" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="7">
+        <v>189</v>
+      </c>
+      <c r="J10" s="7">
+        <v>258</v>
+      </c>
+      <c r="K10" s="7">
+        <f>SUM(K3:K9)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" thickBot="1">
+      <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" thickBot="1">
+      <c r="A12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:11" ht="52" customHeight="1" thickBot="1">
+      <c r="A13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" ht="16" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" ht="16" thickBot="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" ht="16" thickBot="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" ht="44" customHeight="1" thickBot="1">
+      <c r="A17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>